<commit_message>
Added ensemble into write_predictions, Switched back to 3QA with 1 hidden layer
</commit_message>
<xml_diff>
--- a/examples/output/190316-05_33-errors-NoNull_NoEns.xlsx
+++ b/examples/output/190316-05_33-errors-NoNull_NoEns.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klalande/Box Sync/klalande/Kevin/Online Courses/2017 Stanford Graduate Certificate/CS224/02_Project/01_Code/pytorch-pretrained-BERT/examples/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AE8892-E164-174B-9964-5AE4ADBB0874}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0344598D-EB86-0244-BC7B-EDF36511C73C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="22900" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="errorAnalysis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -152,7 +159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +178,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,12 +225,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AC466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -816,6 +831,22 @@
       </c>
     </row>
     <row r="15" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="D15" s="3">
+        <f>SUM(D13:D14)</f>
+        <v>1381</v>
+      </c>
+      <c r="E15" s="3">
+        <f>SUM(E13:E14)</f>
+        <v>4371</v>
+      </c>
+      <c r="F15" s="3">
+        <f>SUM(F13:F14)</f>
+        <v>326</v>
+      </c>
+      <c r="G15" s="3">
+        <f>SUM(G13:G14)</f>
+        <v>6078</v>
+      </c>
       <c r="K15" s="1">
         <v>217</v>
       </c>

</xml_diff>